<commit_message>
set default object for all job and level
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/InitProperty.xlsx
+++ b/_Out/NFDataCfg/Excel/InitProperty.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uowou\Desktop\NFGameDemo\NoahFrame\_Out\NFDataCfg\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5F9A17-15FE-4793-8E53-4B4A8C3762DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="23360"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="215">
   <si>
     <t>Id</t>
   </si>
@@ -67,9 +73,6 @@
     <t>InitProperty1</t>
   </si>
   <si>
-    <t>Hero001</t>
-  </si>
-  <si>
     <t>InitProperty2</t>
   </si>
   <si>
@@ -659,19 +662,16 @@
   </si>
   <si>
     <t>InitProperty198</t>
+  </si>
+  <si>
+    <t>DefaultObject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,152 +700,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -870,194 +726,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1181,251 +851,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1476,61 +904,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1788,29 +1172,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="10" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.203125" customWidth="1"/>
-    <col min="2" max="2" width="7.203125" customWidth="1"/>
-    <col min="3" max="3" width="9.3359375" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" customWidth="1"/>
+    <col min="2" max="2" width="7.19921875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="30.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1824,7 +1207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:4">
+    <row r="2" spans="1:4" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1838,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:4">
+    <row r="3" spans="1:4" s="2" customFormat="1">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1852,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:4">
+    <row r="4" spans="1:4" s="2" customFormat="1">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1866,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:4">
+    <row r="5" spans="1:4" s="2" customFormat="1">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1880,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:4">
+    <row r="6" spans="1:4" s="2" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1894,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:4">
+    <row r="7" spans="1:4" s="3" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -1904,11 +1287,11 @@
       <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:4">
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="13.5">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1922,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:4">
+    <row r="9" spans="1:4" s="3" customFormat="1" ht="13.5">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1936,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="17.75" spans="1:4">
+    <row r="10" spans="1:4" s="4" customFormat="1">
       <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
@@ -1946,7 +1329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="17.55" spans="1:4">
+    <row r="11" spans="1:4">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1957,12 +1340,12 @@
         <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="12" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="12" ht="17.55" spans="1:4">
-      <c r="A12" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="B12" s="13">
         <v>0</v>
@@ -1971,12 +1354,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="13">
         <v>0</v>
@@ -1985,12 +1368,12 @@
         <v>3</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="13">
         <v>0</v>
@@ -1999,12 +1382,12 @@
         <v>4</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="13">
         <v>0</v>
@@ -2013,12 +1396,12 @@
         <v>5</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
@@ -2027,12 +1410,12 @@
         <v>6</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
@@ -2041,12 +1424,12 @@
         <v>7</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="13">
         <v>0</v>
@@ -2055,12 +1438,12 @@
         <v>8</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="13">
         <v>0</v>
@@ -2069,12 +1452,12 @@
         <v>9</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="13">
         <v>0</v>
@@ -2083,12 +1466,12 @@
         <v>10</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="13">
         <v>0</v>
@@ -2097,12 +1480,12 @@
         <v>11</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="13">
         <v>0</v>
@@ -2111,12 +1494,12 @@
         <v>12</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="13">
         <v>0</v>
@@ -2125,12 +1508,12 @@
         <v>13</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="13">
         <v>0</v>
@@ -2139,12 +1522,12 @@
         <v>14</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="13">
         <v>0</v>
@@ -2153,12 +1536,12 @@
         <v>15</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="13">
         <v>0</v>
@@ -2167,12 +1550,12 @@
         <v>16</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="13">
         <v>0</v>
@@ -2181,12 +1564,12 @@
         <v>17</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="13">
         <v>0</v>
@@ -2195,12 +1578,12 @@
         <v>18</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="13">
         <v>0</v>
@@ -2209,12 +1592,12 @@
         <v>19</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="13">
         <v>0</v>
@@ -2223,12 +1606,12 @@
         <v>20</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="13">
         <v>0</v>
@@ -2237,12 +1620,12 @@
         <v>21</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="13">
         <v>0</v>
@@ -2251,12 +1634,12 @@
         <v>22</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="13">
         <v>0</v>
@@ -2265,12 +1648,12 @@
         <v>23</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="13">
         <v>0</v>
@@ -2279,12 +1662,12 @@
         <v>24</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="13">
         <v>0</v>
@@ -2293,12 +1676,12 @@
         <v>25</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="13">
         <v>0</v>
@@ -2307,12 +1690,12 @@
         <v>26</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="13">
         <v>0</v>
@@ -2321,12 +1704,12 @@
         <v>27</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="13">
         <v>0</v>
@@ -2335,12 +1718,12 @@
         <v>28</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="13">
         <v>0</v>
@@ -2349,12 +1732,12 @@
         <v>29</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="13">
         <v>0</v>
@@ -2363,12 +1746,12 @@
         <v>30</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="13">
         <v>0</v>
@@ -2377,12 +1760,12 @@
         <v>31</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" s="13">
         <v>0</v>
@@ -2391,12 +1774,12 @@
         <v>32</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="13">
         <v>0</v>
@@ -2405,12 +1788,12 @@
         <v>33</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="13">
         <v>0</v>
@@ -2419,12 +1802,12 @@
         <v>34</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="13">
         <v>0</v>
@@ -2433,12 +1816,12 @@
         <v>35</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" s="13">
         <v>0</v>
@@ -2447,12 +1830,12 @@
         <v>36</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="13">
         <v>0</v>
@@ -2461,12 +1844,12 @@
         <v>37</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="13">
         <v>0</v>
@@ -2475,12 +1858,12 @@
         <v>38</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" s="13">
         <v>0</v>
@@ -2489,12 +1872,12 @@
         <v>39</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="13">
         <v>0</v>
@@ -2503,12 +1886,12 @@
         <v>40</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" s="13">
         <v>0</v>
@@ -2517,12 +1900,12 @@
         <v>41</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="13">
         <v>0</v>
@@ -2531,12 +1914,12 @@
         <v>42</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" s="13">
         <v>0</v>
@@ -2545,12 +1928,12 @@
         <v>43</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" s="13">
         <v>0</v>
@@ -2559,12 +1942,12 @@
         <v>44</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" s="13">
         <v>0</v>
@@ -2573,12 +1956,12 @@
         <v>45</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="13">
         <v>0</v>
@@ -2587,12 +1970,12 @@
         <v>46</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="13">
         <v>0</v>
@@ -2601,12 +1984,12 @@
         <v>47</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" s="13">
         <v>0</v>
@@ -2615,12 +1998,12 @@
         <v>48</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" s="13">
         <v>0</v>
@@ -2629,12 +2012,12 @@
         <v>49</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" s="13">
         <v>0</v>
@@ -2643,12 +2026,12 @@
         <v>50</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" s="13">
         <v>0</v>
@@ -2657,12 +2040,12 @@
         <v>51</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" s="13">
         <v>0</v>
@@ -2671,12 +2054,12 @@
         <v>52</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="13">
         <v>0</v>
@@ -2685,12 +2068,12 @@
         <v>53</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" s="13">
         <v>0</v>
@@ -2699,12 +2082,12 @@
         <v>54</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" s="13">
         <v>0</v>
@@ -2713,12 +2096,12 @@
         <v>55</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B66" s="13">
         <v>0</v>
@@ -2727,12 +2110,12 @@
         <v>56</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="13">
         <v>0</v>
@@ -2741,12 +2124,12 @@
         <v>57</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" s="13">
         <v>0</v>
@@ -2755,12 +2138,12 @@
         <v>58</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" s="13">
         <v>0</v>
@@ -2769,12 +2152,12 @@
         <v>59</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="13">
         <v>0</v>
@@ -2783,12 +2166,12 @@
         <v>60</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="13">
         <v>0</v>
@@ -2797,12 +2180,12 @@
         <v>61</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="13">
         <v>0</v>
@@ -2811,12 +2194,12 @@
         <v>62</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="13">
         <v>0</v>
@@ -2825,12 +2208,12 @@
         <v>63</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B74" s="13">
         <v>0</v>
@@ -2839,12 +2222,12 @@
         <v>64</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="13">
         <v>0</v>
@@ -2853,12 +2236,12 @@
         <v>65</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B76" s="13">
         <v>0</v>
@@ -2867,12 +2250,12 @@
         <v>66</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="77" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B77" s="13">
         <v>0</v>
@@ -2881,12 +2264,12 @@
         <v>67</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B78" s="13">
         <v>0</v>
@@ -2895,12 +2278,12 @@
         <v>68</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="79" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79" s="13">
         <v>0</v>
@@ -2909,12 +2292,12 @@
         <v>69</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="80" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B80" s="13">
         <v>0</v>
@@ -2923,12 +2306,12 @@
         <v>70</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" ht="15" customHeight="1" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B81" s="13">
         <v>0</v>
@@ -2937,12 +2320,12 @@
         <v>71</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="82" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82" s="13">
         <v>0</v>
@@ -2951,12 +2334,12 @@
         <v>72</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="83" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B83" s="13">
         <v>0</v>
@@ -2965,12 +2348,12 @@
         <v>73</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="84" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" s="13">
         <v>0</v>
@@ -2979,12 +2362,12 @@
         <v>74</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="85" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85" s="13">
         <v>0</v>
@@ -2993,12 +2376,12 @@
         <v>75</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="86" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B86" s="13">
         <v>0</v>
@@ -3007,12 +2390,12 @@
         <v>76</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="87" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B87" s="13">
         <v>0</v>
@@ -3021,12 +2404,12 @@
         <v>77</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B88" s="13">
         <v>0</v>
@@ -3035,12 +2418,12 @@
         <v>78</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="89" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B89" s="13">
         <v>0</v>
@@ -3049,12 +2432,12 @@
         <v>79</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="90" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B90" s="13">
         <v>0</v>
@@ -3063,12 +2446,12 @@
         <v>80</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B91" s="13">
         <v>0</v>
@@ -3077,12 +2460,12 @@
         <v>81</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="92" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B92" s="13">
         <v>0</v>
@@ -3091,12 +2474,12 @@
         <v>82</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="93" ht="15" customHeight="1" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1">
       <c r="A93" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B93" s="13">
         <v>0</v>
@@ -3105,12 +2488,12 @@
         <v>83</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="94" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B94" s="13">
         <v>0</v>
@@ -3119,12 +2502,12 @@
         <v>84</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="95" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B95" s="13">
         <v>0</v>
@@ -3133,12 +2516,12 @@
         <v>85</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="96" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B96" s="13">
         <v>0</v>
@@ -3147,12 +2530,12 @@
         <v>86</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="97" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="13">
         <v>0</v>
@@ -3161,12 +2544,12 @@
         <v>87</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B98" s="13">
         <v>0</v>
@@ -3175,12 +2558,12 @@
         <v>88</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B99" s="13">
         <v>0</v>
@@ -3189,12 +2572,12 @@
         <v>89</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B100" s="13">
         <v>0</v>
@@ -3203,12 +2586,12 @@
         <v>90</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="101" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B101" s="13">
         <v>0</v>
@@ -3217,12 +2600,12 @@
         <v>91</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="102" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B102" s="13">
         <v>0</v>
@@ -3231,12 +2614,12 @@
         <v>92</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="103" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B103" s="13">
         <v>0</v>
@@ -3245,12 +2628,12 @@
         <v>93</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="104" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B104" s="13">
         <v>0</v>
@@ -3259,12 +2642,12 @@
         <v>94</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" ht="15" customHeight="1" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="A105" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B105" s="13">
         <v>0</v>
@@ -3273,12 +2656,12 @@
         <v>95</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B106" s="13">
         <v>0</v>
@@ -3287,12 +2670,12 @@
         <v>96</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="107" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107" s="13">
         <v>0</v>
@@ -3301,12 +2684,12 @@
         <v>97</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="108" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B108" s="13">
         <v>0</v>
@@ -3315,12 +2698,12 @@
         <v>98</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="109" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B109" s="13">
         <v>0</v>
@@ -3329,26 +2712,26 @@
         <v>99</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="110" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="13">
+        <v>1</v>
+      </c>
+      <c r="C110" s="13">
+        <v>1</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="B110" s="13">
-        <v>1</v>
-      </c>
-      <c r="C110" s="13">
-        <v>1</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="111" ht="17.55" spans="1:4">
-      <c r="A111" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="B111" s="13">
         <v>1</v>
@@ -3357,12 +2740,12 @@
         <v>2</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="112" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" s="13">
         <v>1</v>
@@ -3371,12 +2754,12 @@
         <v>3</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="113" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113" s="13">
         <v>1</v>
@@ -3385,12 +2768,12 @@
         <v>4</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="114" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114" s="13">
         <v>1</v>
@@ -3399,12 +2782,12 @@
         <v>5</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="115" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115" s="13">
         <v>1</v>
@@ -3413,12 +2796,12 @@
         <v>6</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="116" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B116" s="13">
         <v>1</v>
@@ -3427,12 +2810,12 @@
         <v>7</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="117" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B117" s="13">
         <v>1</v>
@@ -3441,12 +2824,12 @@
         <v>8</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="118" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B118" s="13">
         <v>1</v>
@@ -3455,12 +2838,12 @@
         <v>9</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="119" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B119" s="13">
         <v>1</v>
@@ -3469,12 +2852,12 @@
         <v>10</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="120" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B120" s="13">
         <v>1</v>
@@ -3483,12 +2866,12 @@
         <v>11</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="121" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B121" s="13">
         <v>1</v>
@@ -3497,12 +2880,12 @@
         <v>12</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="122" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B122" s="13">
         <v>1</v>
@@ -3511,12 +2894,12 @@
         <v>13</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="123" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B123" s="13">
         <v>1</v>
@@ -3525,12 +2908,12 @@
         <v>14</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="124" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B124" s="13">
         <v>1</v>
@@ -3539,12 +2922,12 @@
         <v>15</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="125" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B125" s="13">
         <v>1</v>
@@ -3553,12 +2936,12 @@
         <v>16</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="126" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B126" s="13">
         <v>1</v>
@@ -3567,12 +2950,12 @@
         <v>17</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="127" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B127" s="13">
         <v>1</v>
@@ -3581,12 +2964,12 @@
         <v>18</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="128" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B128" s="13">
         <v>1</v>
@@ -3595,12 +2978,12 @@
         <v>19</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="129" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B129" s="13">
         <v>1</v>
@@ -3609,12 +2992,12 @@
         <v>20</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="130" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B130" s="13">
         <v>1</v>
@@ -3623,12 +3006,12 @@
         <v>21</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="131" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B131" s="13">
         <v>1</v>
@@ -3637,12 +3020,12 @@
         <v>22</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="132" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132" s="13">
         <v>1</v>
@@ -3651,12 +3034,12 @@
         <v>23</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="133" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B133" s="13">
         <v>1</v>
@@ -3665,12 +3048,12 @@
         <v>24</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="134" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B134" s="13">
         <v>1</v>
@@ -3679,12 +3062,12 @@
         <v>25</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="135" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B135" s="13">
         <v>1</v>
@@ -3693,12 +3076,12 @@
         <v>26</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="136" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B136" s="13">
         <v>1</v>
@@ -3707,12 +3090,12 @@
         <v>27</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="137" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B137" s="13">
         <v>1</v>
@@ -3721,12 +3104,12 @@
         <v>28</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="138" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B138" s="13">
         <v>1</v>
@@ -3735,12 +3118,12 @@
         <v>29</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="139" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B139" s="13">
         <v>1</v>
@@ -3749,12 +3132,12 @@
         <v>30</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="140" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B140" s="13">
         <v>1</v>
@@ -3763,12 +3146,12 @@
         <v>31</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="141" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B141" s="13">
         <v>1</v>
@@ -3777,12 +3160,12 @@
         <v>32</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="142" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B142" s="13">
         <v>1</v>
@@ -3791,12 +3174,12 @@
         <v>33</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="143" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B143" s="13">
         <v>1</v>
@@ -3805,12 +3188,12 @@
         <v>34</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="144" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B144" s="13">
         <v>1</v>
@@ -3819,12 +3202,12 @@
         <v>35</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="145" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B145" s="13">
         <v>1</v>
@@ -3833,12 +3216,12 @@
         <v>36</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="146" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B146" s="13">
         <v>1</v>
@@ -3847,12 +3230,12 @@
         <v>37</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="147" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B147" s="13">
         <v>1</v>
@@ -3861,12 +3244,12 @@
         <v>38</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="148" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B148" s="13">
         <v>1</v>
@@ -3875,12 +3258,12 @@
         <v>39</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="149" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B149" s="13">
         <v>1</v>
@@ -3889,12 +3272,12 @@
         <v>40</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="150" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B150" s="13">
         <v>1</v>
@@ -3903,12 +3286,12 @@
         <v>41</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="151" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B151" s="13">
         <v>1</v>
@@ -3917,12 +3300,12 @@
         <v>42</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="152" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B152" s="13">
         <v>1</v>
@@ -3931,12 +3314,12 @@
         <v>43</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="153" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B153" s="13">
         <v>1</v>
@@ -3945,12 +3328,12 @@
         <v>44</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="154" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B154" s="13">
         <v>1</v>
@@ -3959,12 +3342,12 @@
         <v>45</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="155" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B155" s="13">
         <v>1</v>
@@ -3973,12 +3356,12 @@
         <v>46</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="156" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B156" s="13">
         <v>1</v>
@@ -3987,12 +3370,12 @@
         <v>47</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="157" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B157" s="13">
         <v>1</v>
@@ -4001,12 +3384,12 @@
         <v>48</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="158" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B158" s="13">
         <v>1</v>
@@ -4015,12 +3398,12 @@
         <v>49</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="159" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B159" s="13">
         <v>1</v>
@@ -4029,12 +3412,12 @@
         <v>50</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="160" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B160" s="13">
         <v>1</v>
@@ -4043,12 +3426,12 @@
         <v>51</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="161" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B161" s="13">
         <v>1</v>
@@ -4057,12 +3440,12 @@
         <v>52</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="162" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B162" s="13">
         <v>1</v>
@@ -4071,12 +3454,12 @@
         <v>53</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B163" s="13">
         <v>1</v>
@@ -4085,12 +3468,12 @@
         <v>54</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="164" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B164" s="13">
         <v>1</v>
@@ -4099,12 +3482,12 @@
         <v>55</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="165" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B165" s="13">
         <v>1</v>
@@ -4113,12 +3496,12 @@
         <v>56</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="166" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B166" s="13">
         <v>1</v>
@@ -4127,12 +3510,12 @@
         <v>57</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="167" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B167" s="13">
         <v>1</v>
@@ -4141,12 +3524,12 @@
         <v>58</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="168" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B168" s="13">
         <v>1</v>
@@ -4155,12 +3538,12 @@
         <v>59</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="169" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B169" s="13">
         <v>1</v>
@@ -4169,12 +3552,12 @@
         <v>60</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="170" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B170" s="13">
         <v>1</v>
@@ -4183,12 +3566,12 @@
         <v>61</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="171" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B171" s="13">
         <v>1</v>
@@ -4197,12 +3580,12 @@
         <v>62</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="172" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B172" s="13">
         <v>1</v>
@@ -4211,12 +3594,12 @@
         <v>63</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="173" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B173" s="13">
         <v>1</v>
@@ -4225,12 +3608,12 @@
         <v>64</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="174" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B174" s="13">
         <v>1</v>
@@ -4239,12 +3622,12 @@
         <v>65</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="175" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B175" s="13">
         <v>1</v>
@@ -4253,12 +3636,12 @@
         <v>66</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="176" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B176" s="13">
         <v>1</v>
@@ -4267,12 +3650,12 @@
         <v>67</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="177" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B177" s="13">
         <v>1</v>
@@ -4281,12 +3664,12 @@
         <v>68</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="178" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B178" s="13">
         <v>1</v>
@@ -4295,12 +3678,12 @@
         <v>69</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="179" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B179" s="13">
         <v>1</v>
@@ -4309,12 +3692,12 @@
         <v>70</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="180" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B180" s="13">
         <v>1</v>
@@ -4323,12 +3706,12 @@
         <v>71</v>
       </c>
       <c r="D180" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="181" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B181" s="13">
         <v>1</v>
@@ -4337,12 +3720,12 @@
         <v>72</v>
       </c>
       <c r="D181" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="182" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B182" s="13">
         <v>1</v>
@@ -4351,12 +3734,12 @@
         <v>73</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="183" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B183" s="13">
         <v>1</v>
@@ -4365,12 +3748,12 @@
         <v>74</v>
       </c>
       <c r="D183" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="184" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B184" s="13">
         <v>1</v>
@@ -4379,12 +3762,12 @@
         <v>75</v>
       </c>
       <c r="D184" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="185" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B185" s="13">
         <v>1</v>
@@ -4393,12 +3776,12 @@
         <v>76</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="186" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B186" s="13">
         <v>1</v>
@@ -4407,12 +3790,12 @@
         <v>77</v>
       </c>
       <c r="D186" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="187" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B187" s="13">
         <v>1</v>
@@ -4421,12 +3804,12 @@
         <v>78</v>
       </c>
       <c r="D187" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="188" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B188" s="13">
         <v>1</v>
@@ -4435,12 +3818,12 @@
         <v>79</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="189" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B189" s="13">
         <v>1</v>
@@ -4449,12 +3832,12 @@
         <v>80</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="190" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B190" s="13">
         <v>1</v>
@@ -4463,12 +3846,12 @@
         <v>81</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="191" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B191" s="13">
         <v>1</v>
@@ -4477,12 +3860,12 @@
         <v>82</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="192" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B192" s="13">
         <v>1</v>
@@ -4491,12 +3874,12 @@
         <v>83</v>
       </c>
       <c r="D192" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="193" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
       <c r="A193" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B193" s="13">
         <v>1</v>
@@ -4505,12 +3888,12 @@
         <v>84</v>
       </c>
       <c r="D193" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="194" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
       <c r="A194" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B194" s="13">
         <v>1</v>
@@ -4519,12 +3902,12 @@
         <v>85</v>
       </c>
       <c r="D194" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="195" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B195" s="13">
         <v>1</v>
@@ -4533,12 +3916,12 @@
         <v>86</v>
       </c>
       <c r="D195" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="196" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
       <c r="A196" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B196" s="13">
         <v>1</v>
@@ -4547,12 +3930,12 @@
         <v>87</v>
       </c>
       <c r="D196" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="197" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
       <c r="A197" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B197" s="13">
         <v>1</v>
@@ -4561,12 +3944,12 @@
         <v>88</v>
       </c>
       <c r="D197" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="198" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
       <c r="A198" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B198" s="13">
         <v>1</v>
@@ -4575,12 +3958,12 @@
         <v>89</v>
       </c>
       <c r="D198" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="199" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
       <c r="A199" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B199" s="13">
         <v>1</v>
@@ -4589,12 +3972,12 @@
         <v>90</v>
       </c>
       <c r="D199" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="200" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
       <c r="A200" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B200" s="13">
         <v>1</v>
@@ -4603,12 +3986,12 @@
         <v>91</v>
       </c>
       <c r="D200" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="201" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
       <c r="A201" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B201" s="13">
         <v>1</v>
@@ -4617,12 +4000,12 @@
         <v>92</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="202" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
       <c r="A202" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B202" s="13">
         <v>1</v>
@@ -4631,12 +4014,12 @@
         <v>93</v>
       </c>
       <c r="D202" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="203" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
       <c r="A203" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B203" s="13">
         <v>1</v>
@@ -4645,12 +4028,12 @@
         <v>94</v>
       </c>
       <c r="D203" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="204" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
       <c r="A204" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B204" s="13">
         <v>1</v>
@@ -4659,12 +4042,12 @@
         <v>95</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="205" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
       <c r="A205" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B205" s="13">
         <v>1</v>
@@ -4673,12 +4056,12 @@
         <v>96</v>
       </c>
       <c r="D205" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="206" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
       <c r="A206" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B206" s="13">
         <v>1</v>
@@ -4687,12 +4070,12 @@
         <v>97</v>
       </c>
       <c r="D206" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="207" ht="17.55" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
       <c r="A207" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B207" s="13">
         <v>1</v>
@@ -4701,12 +4084,12 @@
         <v>98</v>
       </c>
       <c r="D207" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="208" ht="16.8" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
       <c r="A208" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B208" s="13">
         <v>1</v>
@@ -4715,7 +4098,7 @@
         <v>99</v>
       </c>
       <c r="D208" s="14" t="s">
-        <v>17</v>
+        <v>214</v>
       </c>
     </row>
     <row r="209" spans="3:3">
@@ -4726,12 +4109,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C9 D7:H9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C9 E7:H9 D8:D9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
support multiple projects using the same config files
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/InitProperty.xlsx
+++ b/_Out/NFDataCfg/Excel/InitProperty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uowou\Desktop\NFGameDemo\NoahFrame\_Out\NFDataCfg\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5F9A17-15FE-4793-8E53-4B4A8C3762DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133B8761-CA87-4CD5-BC88-10C28AC22536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="37636" windowHeight="20416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="217">
   <si>
     <t>Id</t>
   </si>
@@ -665,13 +665,19 @@
   </si>
   <si>
     <t>DefaultObject</t>
+  </si>
+  <si>
+    <t>HeroConfigIDEx</t>
+  </si>
+  <si>
+    <t>Hero001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,6 +705,12 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1178,11 +1190,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D210"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="10" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E208" sqref="E208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1190,10 +1202,10 @@
     <col min="1" max="1" width="18.19921875" customWidth="1"/>
     <col min="2" max="2" width="7.19921875" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.796875" customWidth="1"/>
+    <col min="4" max="5" width="30.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1206,8 +1218,11 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="E1" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1220,8 +1235,11 @@
       <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1">
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1234,8 +1252,11 @@
       <c r="D3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1">
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1248,8 +1269,11 @@
       <c r="D4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1">
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1262,8 +1286,11 @@
       <c r="D5" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1">
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1276,8 +1303,11 @@
       <c r="D6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1">
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -1290,8 +1320,11 @@
       <c r="D7" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="13.5">
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="13.5">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1304,8 +1337,11 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" ht="13.5">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="13.5">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1318,8 +1354,11 @@
       <c r="D9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="4" customFormat="1" ht="14.65" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
@@ -1328,8 +1367,11 @@
       <c r="D10" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.65" thickBot="1">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1342,8 +1384,11 @@
       <c r="D11" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.65" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -1356,8 +1401,11 @@
       <c r="D12" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.65" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -1370,8 +1418,11 @@
       <c r="D13" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.65" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -1384,8 +1435,11 @@
       <c r="D14" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.65" thickBot="1">
       <c r="A15" s="12" t="s">
         <v>20</v>
       </c>
@@ -1398,8 +1452,11 @@
       <c r="D15" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.65" thickBot="1">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
@@ -1412,8 +1469,11 @@
       <c r="D16" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.65" thickBot="1">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1426,8 +1486,11 @@
       <c r="D17" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.65" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -1440,8 +1503,11 @@
       <c r="D18" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.65" thickBot="1">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
@@ -1454,8 +1520,11 @@
       <c r="D19" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.65" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1468,8 +1537,11 @@
       <c r="D20" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.65" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -1482,8 +1554,11 @@
       <c r="D21" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.65" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -1496,8 +1571,11 @@
       <c r="D22" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.65" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -1510,8 +1588,11 @@
       <c r="D23" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.65" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1524,8 +1605,11 @@
       <c r="D24" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.65" thickBot="1">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -1538,8 +1622,11 @@
       <c r="D25" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.65" thickBot="1">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -1552,8 +1639,11 @@
       <c r="D26" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.65" thickBot="1">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1566,8 +1656,11 @@
       <c r="D27" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.65" thickBot="1">
       <c r="A28" s="12" t="s">
         <v>33</v>
       </c>
@@ -1580,8 +1673,11 @@
       <c r="D28" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.65" thickBot="1">
       <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
@@ -1594,8 +1690,11 @@
       <c r="D29" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.65" thickBot="1">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -1608,8 +1707,11 @@
       <c r="D30" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.65" thickBot="1">
       <c r="A31" s="12" t="s">
         <v>36</v>
       </c>
@@ -1622,8 +1724,11 @@
       <c r="D31" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.65" thickBot="1">
       <c r="A32" s="12" t="s">
         <v>37</v>
       </c>
@@ -1636,8 +1741,11 @@
       <c r="D32" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.65" thickBot="1">
       <c r="A33" s="12" t="s">
         <v>38</v>
       </c>
@@ -1650,8 +1758,11 @@
       <c r="D33" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.65" thickBot="1">
       <c r="A34" s="12" t="s">
         <v>39</v>
       </c>
@@ -1664,8 +1775,11 @@
       <c r="D34" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.65" thickBot="1">
       <c r="A35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1678,8 +1792,11 @@
       <c r="D35" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.65" thickBot="1">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
@@ -1692,8 +1809,11 @@
       <c r="D36" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.65" thickBot="1">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
@@ -1706,8 +1826,11 @@
       <c r="D37" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.65" thickBot="1">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
@@ -1720,8 +1843,11 @@
       <c r="D38" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.65" thickBot="1">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
@@ -1734,8 +1860,11 @@
       <c r="D39" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.65" thickBot="1">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
@@ -1748,8 +1877,11 @@
       <c r="D40" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.65" thickBot="1">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
@@ -1762,8 +1894,11 @@
       <c r="D41" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.65" thickBot="1">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
@@ -1776,8 +1911,11 @@
       <c r="D42" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.65" thickBot="1">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
@@ -1790,8 +1928,11 @@
       <c r="D43" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.65" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -1804,8 +1945,11 @@
       <c r="D44" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.65" thickBot="1">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -1818,8 +1962,11 @@
       <c r="D45" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.65" thickBot="1">
       <c r="A46" s="12" t="s">
         <v>51</v>
       </c>
@@ -1832,8 +1979,11 @@
       <c r="D46" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.65" thickBot="1">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
@@ -1846,8 +1996,11 @@
       <c r="D47" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.65" thickBot="1">
       <c r="A48" s="12" t="s">
         <v>53</v>
       </c>
@@ -1860,8 +2013,11 @@
       <c r="D48" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.65" thickBot="1">
       <c r="A49" s="12" t="s">
         <v>54</v>
       </c>
@@ -1874,8 +2030,11 @@
       <c r="D49" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.65" thickBot="1">
       <c r="A50" s="12" t="s">
         <v>55</v>
       </c>
@@ -1888,8 +2047,11 @@
       <c r="D50" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.65" thickBot="1">
       <c r="A51" s="12" t="s">
         <v>56</v>
       </c>
@@ -1902,8 +2064,11 @@
       <c r="D51" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.65" thickBot="1">
       <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
@@ -1916,8 +2081,11 @@
       <c r="D52" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.65" thickBot="1">
       <c r="A53" s="12" t="s">
         <v>58</v>
       </c>
@@ -1930,8 +2098,11 @@
       <c r="D53" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.65" thickBot="1">
       <c r="A54" s="12" t="s">
         <v>59</v>
       </c>
@@ -1944,8 +2115,11 @@
       <c r="D54" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.65" thickBot="1">
       <c r="A55" s="12" t="s">
         <v>60</v>
       </c>
@@ -1958,8 +2132,11 @@
       <c r="D55" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.65" thickBot="1">
       <c r="A56" s="12" t="s">
         <v>61</v>
       </c>
@@ -1972,8 +2149,11 @@
       <c r="D56" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.65" thickBot="1">
       <c r="A57" s="12" t="s">
         <v>62</v>
       </c>
@@ -1986,8 +2166,11 @@
       <c r="D57" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.65" thickBot="1">
       <c r="A58" s="12" t="s">
         <v>63</v>
       </c>
@@ -2000,8 +2183,11 @@
       <c r="D58" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.65" thickBot="1">
       <c r="A59" s="12" t="s">
         <v>64</v>
       </c>
@@ -2014,8 +2200,11 @@
       <c r="D59" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.65" thickBot="1">
       <c r="A60" s="12" t="s">
         <v>65</v>
       </c>
@@ -2028,8 +2217,11 @@
       <c r="D60" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.65" thickBot="1">
       <c r="A61" s="12" t="s">
         <v>66</v>
       </c>
@@ -2042,8 +2234,11 @@
       <c r="D61" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="14.65" thickBot="1">
       <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
@@ -2056,8 +2251,11 @@
       <c r="D62" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.65" thickBot="1">
       <c r="A63" s="12" t="s">
         <v>68</v>
       </c>
@@ -2070,8 +2268,11 @@
       <c r="D63" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="14.65" thickBot="1">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -2084,8 +2285,11 @@
       <c r="D64" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.65" thickBot="1">
       <c r="A65" s="12" t="s">
         <v>70</v>
       </c>
@@ -2098,8 +2302,11 @@
       <c r="D65" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="14.65" thickBot="1">
       <c r="A66" s="12" t="s">
         <v>71</v>
       </c>
@@ -2112,8 +2319,11 @@
       <c r="D66" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.65" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>72</v>
       </c>
@@ -2126,8 +2336,11 @@
       <c r="D67" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.65" thickBot="1">
       <c r="A68" s="12" t="s">
         <v>73</v>
       </c>
@@ -2140,8 +2353,11 @@
       <c r="D68" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.65" thickBot="1">
       <c r="A69" s="12" t="s">
         <v>74</v>
       </c>
@@ -2154,8 +2370,11 @@
       <c r="D69" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="14.65" thickBot="1">
       <c r="A70" s="12" t="s">
         <v>75</v>
       </c>
@@ -2168,8 +2387,11 @@
       <c r="D70" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.65" thickBot="1">
       <c r="A71" s="12" t="s">
         <v>76</v>
       </c>
@@ -2182,8 +2404,11 @@
       <c r="D71" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="14.65" thickBot="1">
       <c r="A72" s="12" t="s">
         <v>77</v>
       </c>
@@ -2196,8 +2421,11 @@
       <c r="D72" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.65" thickBot="1">
       <c r="A73" s="12" t="s">
         <v>78</v>
       </c>
@@ -2210,8 +2438,11 @@
       <c r="D73" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="14.65" thickBot="1">
       <c r="A74" s="12" t="s">
         <v>79</v>
       </c>
@@ -2224,8 +2455,11 @@
       <c r="D74" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.65" thickBot="1">
       <c r="A75" s="12" t="s">
         <v>80</v>
       </c>
@@ -2238,8 +2472,11 @@
       <c r="D75" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14.65" thickBot="1">
       <c r="A76" s="12" t="s">
         <v>81</v>
       </c>
@@ -2252,8 +2489,11 @@
       <c r="D76" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="14.65" thickBot="1">
       <c r="A77" s="12" t="s">
         <v>82</v>
       </c>
@@ -2266,8 +2506,11 @@
       <c r="D77" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="14.65" thickBot="1">
       <c r="A78" s="12" t="s">
         <v>83</v>
       </c>
@@ -2280,8 +2523,11 @@
       <c r="D78" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="14.65" thickBot="1">
       <c r="A79" s="12" t="s">
         <v>84</v>
       </c>
@@ -2294,8 +2540,11 @@
       <c r="D79" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="14.65" thickBot="1">
       <c r="A80" s="12" t="s">
         <v>85</v>
       </c>
@@ -2308,8 +2557,11 @@
       <c r="D80" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1">
+      <c r="E80" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15" customHeight="1" thickBot="1">
       <c r="A81" s="12" t="s">
         <v>86</v>
       </c>
@@ -2322,8 +2574,11 @@
       <c r="D81" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="14.65" thickBot="1">
       <c r="A82" s="12" t="s">
         <v>87</v>
       </c>
@@ -2336,8 +2591,11 @@
       <c r="D82" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="14.65" thickBot="1">
       <c r="A83" s="12" t="s">
         <v>88</v>
       </c>
@@ -2350,8 +2608,11 @@
       <c r="D83" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="14.65" thickBot="1">
       <c r="A84" s="12" t="s">
         <v>89</v>
       </c>
@@ -2364,8 +2625,11 @@
       <c r="D84" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="14.65" thickBot="1">
       <c r="A85" s="12" t="s">
         <v>90</v>
       </c>
@@ -2378,8 +2642,11 @@
       <c r="D85" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="14.65" thickBot="1">
       <c r="A86" s="12" t="s">
         <v>91</v>
       </c>
@@ -2392,8 +2659,11 @@
       <c r="D86" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="14.65" thickBot="1">
       <c r="A87" s="12" t="s">
         <v>92</v>
       </c>
@@ -2406,8 +2676,11 @@
       <c r="D87" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="14.65" thickBot="1">
       <c r="A88" s="12" t="s">
         <v>93</v>
       </c>
@@ -2420,8 +2693,11 @@
       <c r="D88" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="14.65" thickBot="1">
       <c r="A89" s="12" t="s">
         <v>94</v>
       </c>
@@ -2434,8 +2710,11 @@
       <c r="D89" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="14.65" thickBot="1">
       <c r="A90" s="12" t="s">
         <v>95</v>
       </c>
@@ -2448,8 +2727,11 @@
       <c r="D90" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="14.65" thickBot="1">
       <c r="A91" s="12" t="s">
         <v>96</v>
       </c>
@@ -2462,8 +2744,11 @@
       <c r="D91" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="14.65" thickBot="1">
       <c r="A92" s="12" t="s">
         <v>97</v>
       </c>
@@ -2476,8 +2761,11 @@
       <c r="D92" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1">
+      <c r="E92" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15" customHeight="1" thickBot="1">
       <c r="A93" s="12" t="s">
         <v>98</v>
       </c>
@@ -2490,8 +2778,11 @@
       <c r="D93" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="14.65" thickBot="1">
       <c r="A94" s="12" t="s">
         <v>99</v>
       </c>
@@ -2504,8 +2795,11 @@
       <c r="D94" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="14.65" thickBot="1">
       <c r="A95" s="12" t="s">
         <v>100</v>
       </c>
@@ -2518,8 +2812,11 @@
       <c r="D95" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="14.65" thickBot="1">
       <c r="A96" s="12" t="s">
         <v>101</v>
       </c>
@@ -2532,8 +2829,11 @@
       <c r="D96" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="14.65" thickBot="1">
       <c r="A97" s="12" t="s">
         <v>102</v>
       </c>
@@ -2546,8 +2846,11 @@
       <c r="D97" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="14.65" thickBot="1">
       <c r="A98" s="12" t="s">
         <v>103</v>
       </c>
@@ -2560,8 +2863,11 @@
       <c r="D98" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="14.65" thickBot="1">
       <c r="A99" s="12" t="s">
         <v>104</v>
       </c>
@@ -2574,8 +2880,11 @@
       <c r="D99" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="14.65" thickBot="1">
       <c r="A100" s="12" t="s">
         <v>105</v>
       </c>
@@ -2588,8 +2897,11 @@
       <c r="D100" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="14.65" thickBot="1">
       <c r="A101" s="12" t="s">
         <v>106</v>
       </c>
@@ -2602,8 +2914,11 @@
       <c r="D101" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="14.65" thickBot="1">
       <c r="A102" s="12" t="s">
         <v>107</v>
       </c>
@@ -2616,8 +2931,11 @@
       <c r="D102" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="14.65" thickBot="1">
       <c r="A103" s="12" t="s">
         <v>108</v>
       </c>
@@ -2630,8 +2948,11 @@
       <c r="D103" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="14.65" thickBot="1">
       <c r="A104" s="12" t="s">
         <v>109</v>
       </c>
@@ -2644,8 +2965,11 @@
       <c r="D104" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1">
+      <c r="E104" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15" customHeight="1" thickBot="1">
       <c r="A105" s="12" t="s">
         <v>110</v>
       </c>
@@ -2658,8 +2982,11 @@
       <c r="D105" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="14.65" thickBot="1">
       <c r="A106" s="12" t="s">
         <v>111</v>
       </c>
@@ -2672,8 +2999,11 @@
       <c r="D106" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="14.65" thickBot="1">
       <c r="A107" s="12" t="s">
         <v>112</v>
       </c>
@@ -2686,8 +3016,11 @@
       <c r="D107" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="14.65" thickBot="1">
       <c r="A108" s="12" t="s">
         <v>113</v>
       </c>
@@ -2700,8 +3033,11 @@
       <c r="D108" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="14.65" thickBot="1">
       <c r="A109" s="12" t="s">
         <v>114</v>
       </c>
@@ -2714,8 +3050,11 @@
       <c r="D109" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="14.65" thickBot="1">
       <c r="A110" s="12" t="s">
         <v>115</v>
       </c>
@@ -2728,8 +3067,11 @@
       <c r="D110" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="14.65" thickBot="1">
       <c r="A111" s="12" t="s">
         <v>116</v>
       </c>
@@ -2742,8 +3084,11 @@
       <c r="D111" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="14.65" thickBot="1">
       <c r="A112" s="12" t="s">
         <v>117</v>
       </c>
@@ -2756,8 +3101,11 @@
       <c r="D112" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="14.65" thickBot="1">
       <c r="A113" s="12" t="s">
         <v>118</v>
       </c>
@@ -2770,8 +3118,11 @@
       <c r="D113" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="14.65" thickBot="1">
       <c r="A114" s="12" t="s">
         <v>119</v>
       </c>
@@ -2784,8 +3135,11 @@
       <c r="D114" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="14.65" thickBot="1">
       <c r="A115" s="12" t="s">
         <v>120</v>
       </c>
@@ -2798,8 +3152,11 @@
       <c r="D115" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="14.65" thickBot="1">
       <c r="A116" s="12" t="s">
         <v>121</v>
       </c>
@@ -2812,8 +3169,11 @@
       <c r="D116" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="14.65" thickBot="1">
       <c r="A117" s="12" t="s">
         <v>122</v>
       </c>
@@ -2826,8 +3186,11 @@
       <c r="D117" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="14.65" thickBot="1">
       <c r="A118" s="12" t="s">
         <v>123</v>
       </c>
@@ -2840,8 +3203,11 @@
       <c r="D118" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="14.65" thickBot="1">
       <c r="A119" s="12" t="s">
         <v>124</v>
       </c>
@@ -2854,8 +3220,11 @@
       <c r="D119" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="14.65" thickBot="1">
       <c r="A120" s="12" t="s">
         <v>125</v>
       </c>
@@ -2868,8 +3237,11 @@
       <c r="D120" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="14.65" thickBot="1">
       <c r="A121" s="12" t="s">
         <v>126</v>
       </c>
@@ -2882,8 +3254,11 @@
       <c r="D121" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="E121" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="14.65" thickBot="1">
       <c r="A122" s="12" t="s">
         <v>127</v>
       </c>
@@ -2896,8 +3271,11 @@
       <c r="D122" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="14.65" thickBot="1">
       <c r="A123" s="12" t="s">
         <v>128</v>
       </c>
@@ -2910,8 +3288,11 @@
       <c r="D123" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="14.65" thickBot="1">
       <c r="A124" s="12" t="s">
         <v>129</v>
       </c>
@@ -2924,8 +3305,11 @@
       <c r="D124" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="14.65" thickBot="1">
       <c r="A125" s="12" t="s">
         <v>130</v>
       </c>
@@ -2938,8 +3322,11 @@
       <c r="D125" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="14.65" thickBot="1">
       <c r="A126" s="12" t="s">
         <v>131</v>
       </c>
@@ -2952,8 +3339,11 @@
       <c r="D126" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="14.65" thickBot="1">
       <c r="A127" s="12" t="s">
         <v>132</v>
       </c>
@@ -2966,8 +3356,11 @@
       <c r="D127" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="14.65" thickBot="1">
       <c r="A128" s="12" t="s">
         <v>133</v>
       </c>
@@ -2980,8 +3373,11 @@
       <c r="D128" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="14.65" thickBot="1">
       <c r="A129" s="12" t="s">
         <v>134</v>
       </c>
@@ -2994,8 +3390,11 @@
       <c r="D129" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="14.65" thickBot="1">
       <c r="A130" s="12" t="s">
         <v>135</v>
       </c>
@@ -3008,8 +3407,11 @@
       <c r="D130" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="14.65" thickBot="1">
       <c r="A131" s="12" t="s">
         <v>136</v>
       </c>
@@ -3022,8 +3424,11 @@
       <c r="D131" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="14.65" thickBot="1">
       <c r="A132" s="12" t="s">
         <v>137</v>
       </c>
@@ -3036,8 +3441,11 @@
       <c r="D132" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="14.65" thickBot="1">
       <c r="A133" s="12" t="s">
         <v>138</v>
       </c>
@@ -3050,8 +3458,11 @@
       <c r="D133" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="14.65" thickBot="1">
       <c r="A134" s="12" t="s">
         <v>139</v>
       </c>
@@ -3064,8 +3475,11 @@
       <c r="D134" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="14.65" thickBot="1">
       <c r="A135" s="12" t="s">
         <v>140</v>
       </c>
@@ -3078,8 +3492,11 @@
       <c r="D135" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="14.65" thickBot="1">
       <c r="A136" s="12" t="s">
         <v>141</v>
       </c>
@@ -3092,8 +3509,11 @@
       <c r="D136" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="14.65" thickBot="1">
       <c r="A137" s="12" t="s">
         <v>142</v>
       </c>
@@ -3106,8 +3526,11 @@
       <c r="D137" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="14.65" thickBot="1">
       <c r="A138" s="12" t="s">
         <v>143</v>
       </c>
@@ -3120,8 +3543,11 @@
       <c r="D138" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="14.65" thickBot="1">
       <c r="A139" s="12" t="s">
         <v>144</v>
       </c>
@@ -3134,8 +3560,11 @@
       <c r="D139" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="14.65" thickBot="1">
       <c r="A140" s="12" t="s">
         <v>145</v>
       </c>
@@ -3148,8 +3577,11 @@
       <c r="D140" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="14.65" thickBot="1">
       <c r="A141" s="12" t="s">
         <v>146</v>
       </c>
@@ -3162,8 +3594,11 @@
       <c r="D141" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="E141" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="14.65" thickBot="1">
       <c r="A142" s="12" t="s">
         <v>147</v>
       </c>
@@ -3176,8 +3611,11 @@
       <c r="D142" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="14.65" thickBot="1">
       <c r="A143" s="12" t="s">
         <v>148</v>
       </c>
@@ -3190,8 +3628,11 @@
       <c r="D143" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="14.65" thickBot="1">
       <c r="A144" s="12" t="s">
         <v>149</v>
       </c>
@@ -3204,8 +3645,11 @@
       <c r="D144" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="14.65" thickBot="1">
       <c r="A145" s="12" t="s">
         <v>150</v>
       </c>
@@ -3218,8 +3662,11 @@
       <c r="D145" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="14.65" thickBot="1">
       <c r="A146" s="12" t="s">
         <v>151</v>
       </c>
@@ -3232,8 +3679,11 @@
       <c r="D146" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="E146" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="14.65" thickBot="1">
       <c r="A147" s="12" t="s">
         <v>152</v>
       </c>
@@ -3246,8 +3696,11 @@
       <c r="D147" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="E147" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="14.65" thickBot="1">
       <c r="A148" s="12" t="s">
         <v>153</v>
       </c>
@@ -3260,8 +3713,11 @@
       <c r="D148" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="E148" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="14.65" thickBot="1">
       <c r="A149" s="12" t="s">
         <v>154</v>
       </c>
@@ -3274,8 +3730,11 @@
       <c r="D149" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="E149" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="14.65" thickBot="1">
       <c r="A150" s="12" t="s">
         <v>155</v>
       </c>
@@ -3288,8 +3747,11 @@
       <c r="D150" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="E150" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="14.65" thickBot="1">
       <c r="A151" s="12" t="s">
         <v>156</v>
       </c>
@@ -3302,8 +3764,11 @@
       <c r="D151" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="E151" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="14.65" thickBot="1">
       <c r="A152" s="12" t="s">
         <v>157</v>
       </c>
@@ -3316,8 +3781,11 @@
       <c r="D152" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="E152" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="14.65" thickBot="1">
       <c r="A153" s="12" t="s">
         <v>158</v>
       </c>
@@ -3330,8 +3798,11 @@
       <c r="D153" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="E153" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="14.65" thickBot="1">
       <c r="A154" s="12" t="s">
         <v>159</v>
       </c>
@@ -3344,8 +3815,11 @@
       <c r="D154" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="E154" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="14.65" thickBot="1">
       <c r="A155" s="12" t="s">
         <v>160</v>
       </c>
@@ -3358,8 +3832,11 @@
       <c r="D155" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="E155" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="14.65" thickBot="1">
       <c r="A156" s="12" t="s">
         <v>161</v>
       </c>
@@ -3372,8 +3849,11 @@
       <c r="D156" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="E156" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="14.65" thickBot="1">
       <c r="A157" s="12" t="s">
         <v>162</v>
       </c>
@@ -3386,8 +3866,11 @@
       <c r="D157" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="E157" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="14.65" thickBot="1">
       <c r="A158" s="12" t="s">
         <v>163</v>
       </c>
@@ -3400,8 +3883,11 @@
       <c r="D158" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="E158" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="14.65" thickBot="1">
       <c r="A159" s="12" t="s">
         <v>164</v>
       </c>
@@ -3414,8 +3900,11 @@
       <c r="D159" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="E159" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="14.65" thickBot="1">
       <c r="A160" s="12" t="s">
         <v>165</v>
       </c>
@@ -3428,8 +3917,11 @@
       <c r="D160" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="E160" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="14.65" thickBot="1">
       <c r="A161" s="12" t="s">
         <v>166</v>
       </c>
@@ -3442,8 +3934,11 @@
       <c r="D161" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="E161" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="14.65" thickBot="1">
       <c r="A162" s="12" t="s">
         <v>167</v>
       </c>
@@ -3456,8 +3951,11 @@
       <c r="D162" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="E162" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="14.65" thickBot="1">
       <c r="A163" s="12" t="s">
         <v>168</v>
       </c>
@@ -3470,8 +3968,11 @@
       <c r="D163" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="E163" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="14.65" thickBot="1">
       <c r="A164" s="12" t="s">
         <v>169</v>
       </c>
@@ -3484,8 +3985,11 @@
       <c r="D164" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="E164" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="14.65" thickBot="1">
       <c r="A165" s="12" t="s">
         <v>170</v>
       </c>
@@ -3498,8 +4002,11 @@
       <c r="D165" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="E165" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="14.65" thickBot="1">
       <c r="A166" s="12" t="s">
         <v>171</v>
       </c>
@@ -3512,8 +4019,11 @@
       <c r="D166" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="E166" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="14.65" thickBot="1">
       <c r="A167" s="12" t="s">
         <v>172</v>
       </c>
@@ -3526,8 +4036,11 @@
       <c r="D167" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="168" spans="1:4">
+      <c r="E167" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="14.65" thickBot="1">
       <c r="A168" s="12" t="s">
         <v>173</v>
       </c>
@@ -3540,8 +4053,11 @@
       <c r="D168" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="169" spans="1:4">
+      <c r="E168" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="14.65" thickBot="1">
       <c r="A169" s="12" t="s">
         <v>174</v>
       </c>
@@ -3554,8 +4070,11 @@
       <c r="D169" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="170" spans="1:4">
+      <c r="E169" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="14.65" thickBot="1">
       <c r="A170" s="12" t="s">
         <v>175</v>
       </c>
@@ -3568,8 +4087,11 @@
       <c r="D170" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="171" spans="1:4">
+      <c r="E170" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="14.65" thickBot="1">
       <c r="A171" s="12" t="s">
         <v>176</v>
       </c>
@@ -3582,8 +4104,11 @@
       <c r="D171" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="172" spans="1:4">
+      <c r="E171" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="14.65" thickBot="1">
       <c r="A172" s="12" t="s">
         <v>177</v>
       </c>
@@ -3596,8 +4121,11 @@
       <c r="D172" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="173" spans="1:4">
+      <c r="E172" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="14.65" thickBot="1">
       <c r="A173" s="12" t="s">
         <v>178</v>
       </c>
@@ -3610,8 +4138,11 @@
       <c r="D173" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="E173" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="14.65" thickBot="1">
       <c r="A174" s="12" t="s">
         <v>179</v>
       </c>
@@ -3624,8 +4155,11 @@
       <c r="D174" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="E174" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="14.65" thickBot="1">
       <c r="A175" s="12" t="s">
         <v>180</v>
       </c>
@@ -3638,8 +4172,11 @@
       <c r="D175" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="E175" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="14.65" thickBot="1">
       <c r="A176" s="12" t="s">
         <v>181</v>
       </c>
@@ -3652,8 +4189,11 @@
       <c r="D176" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="177" spans="1:4">
+      <c r="E176" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="14.65" thickBot="1">
       <c r="A177" s="12" t="s">
         <v>182</v>
       </c>
@@ -3666,8 +4206,11 @@
       <c r="D177" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="178" spans="1:4">
+      <c r="E177" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="14.65" thickBot="1">
       <c r="A178" s="12" t="s">
         <v>183</v>
       </c>
@@ -3680,8 +4223,11 @@
       <c r="D178" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="179" spans="1:4">
+      <c r="E178" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="14.65" thickBot="1">
       <c r="A179" s="12" t="s">
         <v>184</v>
       </c>
@@ -3694,8 +4240,11 @@
       <c r="D179" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="E179" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="14.65" thickBot="1">
       <c r="A180" s="12" t="s">
         <v>185</v>
       </c>
@@ -3708,8 +4257,11 @@
       <c r="D180" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="181" spans="1:4">
+      <c r="E180" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="14.65" thickBot="1">
       <c r="A181" s="12" t="s">
         <v>186</v>
       </c>
@@ -3722,8 +4274,11 @@
       <c r="D181" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="182" spans="1:4">
+      <c r="E181" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="14.65" thickBot="1">
       <c r="A182" s="12" t="s">
         <v>187</v>
       </c>
@@ -3736,8 +4291,11 @@
       <c r="D182" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="183" spans="1:4">
+      <c r="E182" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="14.65" thickBot="1">
       <c r="A183" s="12" t="s">
         <v>188</v>
       </c>
@@ -3750,8 +4308,11 @@
       <c r="D183" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="184" spans="1:4">
+      <c r="E183" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="14.65" thickBot="1">
       <c r="A184" s="12" t="s">
         <v>189</v>
       </c>
@@ -3764,8 +4325,11 @@
       <c r="D184" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="185" spans="1:4">
+      <c r="E184" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="14.65" thickBot="1">
       <c r="A185" s="12" t="s">
         <v>190</v>
       </c>
@@ -3778,8 +4342,11 @@
       <c r="D185" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="186" spans="1:4">
+      <c r="E185" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="14.65" thickBot="1">
       <c r="A186" s="12" t="s">
         <v>191</v>
       </c>
@@ -3792,8 +4359,11 @@
       <c r="D186" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="187" spans="1:4">
+      <c r="E186" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="14.65" thickBot="1">
       <c r="A187" s="12" t="s">
         <v>192</v>
       </c>
@@ -3806,8 +4376,11 @@
       <c r="D187" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="188" spans="1:4">
+      <c r="E187" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="14.65" thickBot="1">
       <c r="A188" s="12" t="s">
         <v>193</v>
       </c>
@@ -3820,8 +4393,11 @@
       <c r="D188" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="189" spans="1:4">
+      <c r="E188" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="14.65" thickBot="1">
       <c r="A189" s="12" t="s">
         <v>194</v>
       </c>
@@ -3834,8 +4410,11 @@
       <c r="D189" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="190" spans="1:4">
+      <c r="E189" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="14.65" thickBot="1">
       <c r="A190" s="12" t="s">
         <v>195</v>
       </c>
@@ -3848,8 +4427,11 @@
       <c r="D190" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="191" spans="1:4">
+      <c r="E190" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="14.65" thickBot="1">
       <c r="A191" s="12" t="s">
         <v>196</v>
       </c>
@@ -3862,8 +4444,11 @@
       <c r="D191" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="192" spans="1:4">
+      <c r="E191" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="14.65" thickBot="1">
       <c r="A192" s="12" t="s">
         <v>197</v>
       </c>
@@ -3876,8 +4461,11 @@
       <c r="D192" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="193" spans="1:4">
+      <c r="E192" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="14.65" thickBot="1">
       <c r="A193" s="12" t="s">
         <v>198</v>
       </c>
@@ -3890,8 +4478,11 @@
       <c r="D193" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="E193" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="14.65" thickBot="1">
       <c r="A194" s="12" t="s">
         <v>199</v>
       </c>
@@ -3904,8 +4495,11 @@
       <c r="D194" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="195" spans="1:4">
+      <c r="E194" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="14.65" thickBot="1">
       <c r="A195" s="12" t="s">
         <v>200</v>
       </c>
@@ -3918,8 +4512,11 @@
       <c r="D195" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="196" spans="1:4">
+      <c r="E195" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="14.65" thickBot="1">
       <c r="A196" s="12" t="s">
         <v>201</v>
       </c>
@@ -3932,8 +4529,11 @@
       <c r="D196" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="197" spans="1:4">
+      <c r="E196" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="14.65" thickBot="1">
       <c r="A197" s="12" t="s">
         <v>202</v>
       </c>
@@ -3946,8 +4546,11 @@
       <c r="D197" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="198" spans="1:4">
+      <c r="E197" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" ht="14.65" thickBot="1">
       <c r="A198" s="12" t="s">
         <v>203</v>
       </c>
@@ -3960,8 +4563,11 @@
       <c r="D198" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="199" spans="1:4">
+      <c r="E198" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="14.65" thickBot="1">
       <c r="A199" s="12" t="s">
         <v>204</v>
       </c>
@@ -3974,8 +4580,11 @@
       <c r="D199" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="200" spans="1:4">
+      <c r="E199" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="14.65" thickBot="1">
       <c r="A200" s="12" t="s">
         <v>205</v>
       </c>
@@ -3988,8 +4597,11 @@
       <c r="D200" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="201" spans="1:4">
+      <c r="E200" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" ht="14.65" thickBot="1">
       <c r="A201" s="12" t="s">
         <v>206</v>
       </c>
@@ -4002,8 +4614,11 @@
       <c r="D201" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="202" spans="1:4">
+      <c r="E201" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="14.65" thickBot="1">
       <c r="A202" s="12" t="s">
         <v>207</v>
       </c>
@@ -4016,8 +4631,11 @@
       <c r="D202" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="203" spans="1:4">
+      <c r="E202" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="14.65" thickBot="1">
       <c r="A203" s="12" t="s">
         <v>208</v>
       </c>
@@ -4030,8 +4648,11 @@
       <c r="D203" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="E203" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="14.65" thickBot="1">
       <c r="A204" s="12" t="s">
         <v>209</v>
       </c>
@@ -4044,8 +4665,11 @@
       <c r="D204" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="205" spans="1:4">
+      <c r="E204" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="14.65" thickBot="1">
       <c r="A205" s="12" t="s">
         <v>210</v>
       </c>
@@ -4058,8 +4682,11 @@
       <c r="D205" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="206" spans="1:4">
+      <c r="E205" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="14.65" thickBot="1">
       <c r="A206" s="12" t="s">
         <v>211</v>
       </c>
@@ -4072,8 +4699,11 @@
       <c r="D206" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="207" spans="1:4">
+      <c r="E206" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="14.65" thickBot="1">
       <c r="A207" s="12" t="s">
         <v>212</v>
       </c>
@@ -4086,8 +4716,11 @@
       <c r="D207" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="208" spans="1:4">
+      <c r="E207" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
       <c r="A208" s="12" t="s">
         <v>213</v>
       </c>
@@ -4100,6 +4733,9 @@
       <c r="D208" s="14" t="s">
         <v>214</v>
       </c>
+      <c r="E208" s="14" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="209" spans="3:3">
       <c r="C209" s="13"/>
@@ -4108,9 +4744,10 @@
       <c r="C210" s="13"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C9 E7:H9 D8:D9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C9 D8:E9 F7:H9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
start more than one threads if we have more than one CPU
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/InitProperty.xlsx
+++ b/_Out/NFDataCfg/Excel/InitProperty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uowou\Desktop\NFGameDemo\NoahFrame\_Out\NFDataCfg\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133B8761-CA87-4CD5-BC88-10C28AC22536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61785AEA-15B7-4738-A99E-BC768A2C4832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="37636" windowHeight="20416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -1194,7 +1194,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E208" sqref="E208"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1321,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" ht="13.5">

</xml_diff>